<commit_message>
Added components in altium library
</commit_message>
<xml_diff>
--- a/hardware/library/Component_Library.xlsx
+++ b/hardware/library/Component_Library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saloni\Documents\LPEDT\project\ecen5833_s22_lpedt_project\hardware\library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55286C47-BB2A-4D05-A076-27B45AFAF9AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{570BFD93-50C1-4259-BD9B-985D0C9E2B0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="369">
   <si>
     <t>Part Description</t>
   </si>
@@ -1093,6 +1093,45 @@
   </si>
   <si>
     <t>P/N:</t>
+  </si>
+  <si>
+    <t>EFR32 Decoupling</t>
+  </si>
+  <si>
+    <t>1uF</t>
+  </si>
+  <si>
+    <t>885012207078 Würth Elektronik | Capacitors | DigiKey</t>
+  </si>
+  <si>
+    <t>885012207078 Datasheet WCAP-CSGP Ceramic Capacitors 0805 (we-online.com)</t>
+  </si>
+  <si>
+    <t>1 µF ±10% 25V Ceramic Capacitor X7R 0805 (2012 Metric)</t>
+  </si>
+  <si>
+    <t>Ferrite bead</t>
+  </si>
+  <si>
+    <t>74279266 Würth Elektronik | Filters | DigiKey</t>
+  </si>
+  <si>
+    <t>74279266 Datasheet WE-CBF SMT EMI Suppression Ferrite Bead (we-online.com)</t>
+  </si>
+  <si>
+    <t>1 kOhms @ 100 MHz 1 Signal Line Ferrite Bead 0603 (1608 Metric) 200mA 600mOhm</t>
+  </si>
+  <si>
+    <t>1 ohm</t>
+  </si>
+  <si>
+    <t>RC0603FR-101RL YAGEO | Resistors | DigiKey</t>
+  </si>
+  <si>
+    <t>PYu-RC_Group_51_RoHS_L_11.pdf (yageo.com)</t>
+  </si>
+  <si>
+    <t>1 Ohms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Thick Film</t>
   </si>
 </sst>
 </file>
@@ -7662,10 +7701,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6443C32-F7E7-4F64-9FFE-AA3B76D48EBB}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -7681,7 +7720,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="50" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>200</v>
       </c>
@@ -7723,7 +7762,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="62.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>203</v>
       </c>
@@ -7737,7 +7776,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="87.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="50" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>204</v>
       </c>
@@ -7751,7 +7790,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="62.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>205</v>
       </c>
@@ -7765,7 +7804,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>206</v>
       </c>
@@ -7787,6 +7826,53 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>208</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>357</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>360</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>358</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="50" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>361</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>364</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>362</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>365</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>368</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>366</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>367</v>
       </c>
     </row>
   </sheetData>
@@ -7805,9 +7891,15 @@
     <hyperlink ref="C8" r:id="rId12" display="https://www.digikey.com/en/products/detail/murata-electronics/GCM1555C1H1R5JA16D/7363196?s=N4IgjCBcoMxaBjKAzAhgGwM4FMA0IB7KAbRACYBWABjgF18AHAFyhAGUmAnASwDsBzEAF98YAGzwQSSGix5CJEDACcYCgA4Q9EM1YceA4fjHLJ02TnxFIpACxVlt8VsYtI7Ln0Ejwy9aegpFAxLBRsQKhcdNw8Db3wyKlsAxGC5K0UwADoKAAIGADEo3XcAVV5uJgB5ZABZbFRMAFdObCMQAFoKMzTQ61IyLR8OwcDpLib5fpBu2iEfUdIEVAZUBEqCTiGgA" xr:uid="{2FD02EB6-154B-4F2F-BBBB-A62C6BF9EA4B}"/>
     <hyperlink ref="C9" r:id="rId13" display="https://www.digikey.com/en/products/detail/samsung-electro-mechanics/RC1005J000CS/3903488" xr:uid="{7C870805-05E3-4AD9-B4DD-72C1547EE639}"/>
     <hyperlink ref="D9" r:id="rId14" display="https://media.digikey.com/pdf/Data Sheets/Samsung PDFs/RC_Series_ds.pdf" xr:uid="{9F258215-1BFD-414D-B1BA-8CB4BBA9AE67}"/>
+    <hyperlink ref="C14" r:id="rId15" display="https://www.digikey.com/en/products/detail/w%C3%BCrth-elektronik/885012207078/5453527" xr:uid="{5B026AA1-D07A-428E-A0DB-AFF5D0AB10F1}"/>
+    <hyperlink ref="D14" r:id="rId16" display="https://www.we-online.com/katalog/datasheet/885012207078.pdf" xr:uid="{6B0C4B17-22AB-41AA-912A-58454578DB1D}"/>
+    <hyperlink ref="C15" r:id="rId17" display="https://www.digikey.com/en/products/detail/w%C3%BCrth-elektronik/74279266/3907315" xr:uid="{34D81E4F-8D35-4700-B752-C6882DC94BC6}"/>
+    <hyperlink ref="D15" r:id="rId18" display="https://www.we-online.com/katalog/datasheet/74279266.pdf" xr:uid="{ADEF27F3-78D7-406E-9F3F-B583592D8660}"/>
+    <hyperlink ref="C16" r:id="rId19" display="https://www.digikey.com/en/products/detail/yageo/RC0603FR-101RL/14286393" xr:uid="{442CE07C-6DF4-4C3B-81AC-1465A64153D0}"/>
+    <hyperlink ref="D16" r:id="rId20" display="https://www.yageo.com/upload/media/product/productsearch/datasheet/rchip/PYu-RC_Group_51_RoHS_L_11.pdf" xr:uid="{6AB09086-52C3-4A0B-A004-D0EA04C3CA9B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId15"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId21"/>
 </worksheet>
 </file>
 
@@ -8838,8 +8930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16CEEC94-12F5-4B70-B3B0-4D2A22D8E1CB}">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>

</xml_diff>